<commit_message>
creating row index and col index dynamically
</commit_message>
<xml_diff>
--- a/data/TestData.xlsx
+++ b/data/TestData.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Mine\Company\NSE\java_selenium_workspace\OrangeHRMAutomation\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Mine\Company\TrainocateApr2022-PWC\eclipse_workspace\OrangeAutomation\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -396,7 +396,7 @@
   <dimension ref="A1:C3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="A2" sqref="A2:C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
demo2-excel to two dim string array
</commit_message>
<xml_diff>
--- a/data/TestData.xlsx
+++ b/data/TestData.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="23">
   <si>
     <t>Username</t>
   </si>
@@ -65,6 +65,36 @@
   </si>
   <si>
     <t>wick</t>
+  </si>
+  <si>
+    <t>Abi</t>
+  </si>
+  <si>
+    <t>admin124</t>
+  </si>
+  <si>
+    <t>admin125</t>
+  </si>
+  <si>
+    <t>admin126</t>
+  </si>
+  <si>
+    <t>admin127</t>
+  </si>
+  <si>
+    <t>admin128</t>
+  </si>
+  <si>
+    <t>admin129</t>
+  </si>
+  <si>
+    <t>admin130</t>
+  </si>
+  <si>
+    <t>admin131</t>
+  </si>
+  <si>
+    <t>admin132</t>
   </si>
 </sst>
 </file>
@@ -393,10 +423,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:C3"/>
+      <selection activeCell="A4" sqref="A4:C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -436,6 +466,116 @@
         <v>3</v>
       </c>
       <c r="C3" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>13</v>
+      </c>
+      <c r="B5" t="s">
+        <v>14</v>
+      </c>
+      <c r="C5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" t="s">
+        <v>15</v>
+      </c>
+      <c r="C6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>13</v>
+      </c>
+      <c r="B11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>13</v>
+      </c>
+      <c r="B13" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" t="s">
         <v>7</v>
       </c>
     </row>

</xml_diff>

<commit_message>
updated common dataprovider for valid,invalid,titlecheck
</commit_message>
<xml_diff>
--- a/data/TestData.xlsx
+++ b/data/TestData.xlsx
@@ -9,12 +9,13 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16125" windowHeight="6180" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16125" windowHeight="6180"/>
   </bookViews>
   <sheets>
     <sheet name="invalidCredentialTest" sheetId="2" r:id="rId1"/>
     <sheet name="validCredentialTest" sheetId="1" r:id="rId2"/>
-    <sheet name="addEmployeeTest" sheetId="3" r:id="rId3"/>
+    <sheet name="validateTitleTest" sheetId="4" r:id="rId3"/>
+    <sheet name="addEmployeeTest" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="0"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="15">
   <si>
     <t>Username</t>
   </si>
@@ -67,34 +68,10 @@
     <t>wick</t>
   </si>
   <si>
-    <t>Abi</t>
-  </si>
-  <si>
-    <t>admin124</t>
-  </si>
-  <si>
-    <t>admin125</t>
-  </si>
-  <si>
-    <t>admin126</t>
-  </si>
-  <si>
-    <t>admin127</t>
-  </si>
-  <si>
-    <t>admin128</t>
-  </si>
-  <si>
-    <t>admin129</t>
-  </si>
-  <si>
-    <t>admin130</t>
-  </si>
-  <si>
-    <t>admin131</t>
-  </si>
-  <si>
-    <t>admin132</t>
+    <t>Title</t>
+  </si>
+  <si>
+    <t>OrangeHRM</t>
   </si>
 </sst>
 </file>
@@ -423,10 +400,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:C13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -469,116 +446,6 @@
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" t="s">
-        <v>3</v>
-      </c>
-      <c r="C4" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" t="s">
-        <v>14</v>
-      </c>
-      <c r="C5" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>13</v>
-      </c>
-      <c r="B6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>13</v>
-      </c>
-      <c r="B7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>13</v>
-      </c>
-      <c r="B8" t="s">
-        <v>17</v>
-      </c>
-      <c r="C8" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>13</v>
-      </c>
-      <c r="B9" t="s">
-        <v>18</v>
-      </c>
-      <c r="C9" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10" t="s">
-        <v>19</v>
-      </c>
-      <c r="C10" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>13</v>
-      </c>
-      <c r="B11" t="s">
-        <v>20</v>
-      </c>
-      <c r="C11" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>13</v>
-      </c>
-      <c r="B12" t="s">
-        <v>21</v>
-      </c>
-      <c r="C12" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>13</v>
-      </c>
-      <c r="B13" t="s">
-        <v>22</v>
-      </c>
-      <c r="C13" t="s">
-        <v>7</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -588,8 +455,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:C3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -641,6 +508,34 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:A2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="11.5703125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C3"/>
   <sheetViews>

</xml_diff>